<commit_message>
Minor Logic Bugs Fixed and Extra Check Logic Added
</commit_message>
<xml_diff>
--- a/BrandexSalesAdapter.ExcelLogic/wwwroot/UploadExcel/TestProducts.xlsx
+++ b/BrandexSalesAdapter.ExcelLogic/wwwroot/UploadExcel/TestProducts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Petar/Documents/Documents – Petar’s MacBook Pro/Firmata/Справка/TestchetaZaSoftware/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Petar/Documents/Documents – Petar’s MacBook Pro/Firmata/Справка/TestForSfotware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5559C5A6-BB59-5E47-8C19-762CFD848E2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1B662F-6D73-9B4E-A219-A9DDFCE98B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="19200" xr2:uid="{16A5BC43-9C9B-884F-97D0-0677DBA8F62A}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{16A5BC43-9C9B-884F-97D0-0677DBA8F62A}"/>
   </bookViews>
   <sheets>
     <sheet name="TestProducts" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>ProductName</t>
   </si>
@@ -210,13 +210,31 @@
   </si>
   <si>
     <t>ЗИН СЕД тб. х 60 - Botanic</t>
+  </si>
+  <si>
+    <t>ВируФор</t>
+  </si>
+  <si>
+    <t>ВФ-60</t>
+  </si>
+  <si>
+    <t>ВИРУФОР тб. х 60</t>
+  </si>
+  <si>
+    <t>Венаксин</t>
+  </si>
+  <si>
+    <t>ВЕ-60</t>
+  </si>
+  <si>
+    <t>ВЕНАКСИН тб. x 60</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -246,8 +264,27 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -260,8 +297,14 @@
         <bgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -271,57 +314,55 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Нормален 2" xfId="1" xr:uid="{4E871DC4-AFAE-8047-853E-AA638A9D43C4}"/>
+    <cellStyle name="Нормален 4" xfId="2" xr:uid="{B3597F04-797B-3D41-8D5F-8384CBEAE784}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -633,488 +674,540 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6851A5F2-561B-A247-B716-A2E5EDA6E350}">
-  <dimension ref="A1:H19"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.5" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
+    <col min="7" max="7" width="37" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2" s="3">
         <v>181111</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>297342</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>3957321</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>50606</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H2" s="1">
-        <v>5</v>
+      <c r="H2" s="6">
+        <v>7.25</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="3">
         <v>181311</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <v>163015</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>3941781</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>48112</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="H3" s="1">
-        <v>5</v>
+      <c r="H3" s="6">
+        <v>7.25</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4" s="3">
         <v>182301</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>175627</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>3941361</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>15267</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="1">
-        <v>7</v>
+      <c r="H4" s="6">
+        <v>9.5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>182501</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>181540</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>3941980</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>15910</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H5" s="1">
-        <v>13.2</v>
+      <c r="H5" s="6">
+        <v>16.25</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>182601</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>229062</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>3947191</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>21887</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="1">
-        <v>13.2</v>
+      <c r="H6" s="7">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="3">
         <v>182701</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="4">
         <v>358144</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E7" s="8">
         <v>3961081</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>15912</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="1">
-        <v>13.2</v>
+      <c r="H7" s="6">
+        <v>16.25</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>182703</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>265299</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>3954833</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>42451</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="H8" s="1">
-        <v>7</v>
+      <c r="H8" s="6">
+        <v>9.5</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>183103</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>216823</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>3956827</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>48446</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="1">
-        <v>5</v>
+      <c r="H9" s="9">
+        <v>7.25</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>183301</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>227070</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>3946611</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>21503</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H10" s="1">
-        <v>13.2</v>
+      <c r="H10" s="6">
+        <v>16.25</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11" s="3">
         <v>183311</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="3">
         <v>236702</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>3947971</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>22885</v>
       </c>
-      <c r="G11" t="s">
+      <c r="G11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="1">
-        <v>4</v>
+      <c r="H11" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="A12" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4">
+      <c r="C12" s="3">
         <v>183501</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="3">
         <v>238262</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>3948008</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>23192</v>
       </c>
-      <c r="G12" t="s">
+      <c r="G12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="1">
-        <v>8.6</v>
+      <c r="H12" s="6">
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="A13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="4">
+      <c r="C13" s="3">
         <v>183701</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="4">
         <v>358150</v>
       </c>
-      <c r="E13" s="7">
+      <c r="E13" s="8">
         <v>3961080</v>
       </c>
-      <c r="F13" s="4">
+      <c r="F13" s="3">
         <v>42094</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="1">
-        <v>13.2</v>
+      <c r="H13" s="6">
+        <v>16.25</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="4">
+      <c r="C14" s="3">
         <v>183901</v>
       </c>
-      <c r="D14" s="4">
+      <c r="D14" s="3">
         <v>294295</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>3956949</v>
       </c>
-      <c r="F14" s="4">
+      <c r="F14" s="3">
         <v>48536</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="H14" s="1">
-        <v>13.2</v>
+      <c r="H14" s="6">
+        <v>16.25</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="A15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="4">
+      <c r="C15" s="3">
         <v>184101</v>
       </c>
-      <c r="D15" s="4">
+      <c r="D15" s="3">
         <v>310887</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>3958154</v>
       </c>
-      <c r="F15" s="4">
+      <c r="F15" s="3">
         <v>51621</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="1">
-        <v>13.2</v>
+      <c r="H15" s="6">
+        <v>16.25</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>184301</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>324487</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>3959302</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>52796</v>
       </c>
-      <c r="G16" t="s">
+      <c r="G16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H16" s="1">
-        <v>10.4</v>
+      <c r="H16" s="6">
+        <v>13.25</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="A17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C17" s="4">
+      <c r="C17" s="3">
         <v>184501</v>
       </c>
-      <c r="D17" s="4">
+      <c r="D17" s="3">
         <v>324493</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>3959303</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F17" s="3">
         <v>52797</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H17" s="1">
-        <v>10.4</v>
+      <c r="H17" s="6">
+        <v>13.25</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="3">
         <v>184701</v>
       </c>
-      <c r="D18" s="8">
+      <c r="D18" s="10">
         <v>368527</v>
       </c>
-      <c r="E18" s="7">
+      <c r="E18" s="8">
         <v>3961353</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="1">
+        <v>57065</v>
+      </c>
       <c r="G18" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="H18" s="1">
-        <v>8.6</v>
+      <c r="H18" s="6">
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H19" s="3"/>
+      <c r="A19" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="2">
+        <v>185101</v>
+      </c>
+      <c r="D19" s="11">
+        <v>376060</v>
+      </c>
+      <c r="E19" s="12">
+        <v>3961844</v>
+      </c>
+      <c r="F19" s="1">
+        <v>57272</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="6">
+        <v>16.25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" s="2">
+        <v>184901</v>
+      </c>
+      <c r="D20" s="2">
+        <v>379229</v>
+      </c>
+      <c r="E20" s="13">
+        <v>3962051</v>
+      </c>
+      <c r="F20" s="1">
+        <v>57672</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H20" s="7">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Sales Logic Fixes + Errors as Array
</commit_message>
<xml_diff>
--- a/BrandexSalesAdapter.ExcelLogic/wwwroot/UploadExcel/TestProducts.xlsx
+++ b/BrandexSalesAdapter.ExcelLogic/wwwroot/UploadExcel/TestProducts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Petar/Documents/Documents – Petar’s MacBook Pro/Firmata/Справка/TestForSfotware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD1B662F-6D73-9B4E-A219-A9DDFCE98B29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8965416B-FB2E-E042-8CB6-FD3C59DF22CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{16A5BC43-9C9B-884F-97D0-0677DBA8F62A}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{16A5BC43-9C9B-884F-97D0-0677DBA8F62A}"/>
   </bookViews>
   <sheets>
     <sheet name="TestProducts" sheetId="1" r:id="rId1"/>
@@ -677,7 +677,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>